<commit_message>
implement of reading data from csv
</commit_message>
<xml_diff>
--- a/InplusTrader/stockBacktest/result/macd/report.xlsx
+++ b/InplusTrader/stockBacktest/result/macd/report.xlsx
@@ -110,7 +110,7 @@
     <t>2016-01-04</t>
   </si>
   <si>
-    <t>/home/vinson/Downloads/InplusTrader-master/InplusTrader/stockBacktest/strategy/macd.py</t>
+    <t>/home/vinson/PycharmProjects/InplusTrader_Linux/InplusTrader/stockBacktest/strategy/macd.py</t>
   </si>
   <si>
     <t>macd</t>
@@ -18635,7 +18635,7 @@
         <v>83.58033600000002</v>
       </c>
       <c r="C2">
-        <v>1492151634</v>
+        <v>1492237712</v>
       </c>
       <c r="D2">
         <v>8.706</v>
@@ -18647,7 +18647,7 @@
         <v>288</v>
       </c>
       <c r="G2">
-        <v>1492151624</v>
+        <v>1492237698</v>
       </c>
       <c r="I2" t="s">
         <v>319</v>
@@ -18673,7 +18673,7 @@
         <v>80.33078399999999</v>
       </c>
       <c r="C3">
-        <v>1492151635</v>
+        <v>1492237713</v>
       </c>
       <c r="D3">
         <v>8.368</v>
@@ -18685,7 +18685,7 @@
         <v>288</v>
       </c>
       <c r="G3">
-        <v>1492151625</v>
+        <v>1492237699</v>
       </c>
       <c r="I3" t="s">
         <v>320</v>
@@ -18711,7 +18711,7 @@
         <v>80.29160159999999</v>
       </c>
       <c r="C4">
-        <v>1492151636</v>
+        <v>1492237714</v>
       </c>
       <c r="D4">
         <v>9.380000000000001</v>
@@ -18723,7 +18723,7 @@
         <v>288</v>
       </c>
       <c r="G4">
-        <v>1492151626</v>
+        <v>1492237700</v>
       </c>
       <c r="I4" t="s">
         <v>319</v>
@@ -18749,7 +18749,7 @@
         <v>72.30730440000001</v>
       </c>
       <c r="C5">
-        <v>1492151637</v>
+        <v>1492237715</v>
       </c>
       <c r="D5">
         <v>8.446999999999999</v>
@@ -18761,7 +18761,7 @@
         <v>288</v>
       </c>
       <c r="G5">
-        <v>1492151627</v>
+        <v>1492237701</v>
       </c>
       <c r="I5" t="s">
         <v>320</v>
@@ -18787,7 +18787,7 @@
         <v>71.12953680000001</v>
       </c>
       <c r="C6">
-        <v>1492151638</v>
+        <v>1492237716</v>
       </c>
       <c r="D6">
         <v>9.459</v>
@@ -18799,7 +18799,7 @@
         <v>288</v>
       </c>
       <c r="G6">
-        <v>1492151628</v>
+        <v>1492237702</v>
       </c>
       <c r="I6" t="s">
         <v>319</v>
@@ -18825,7 +18825,7 @@
         <v>62.6293048</v>
       </c>
       <c r="C7">
-        <v>1492151639</v>
+        <v>1492237717</v>
       </c>
       <c r="D7">
         <v>8.327999999999999</v>
@@ -18837,7 +18837,7 @@
         <v>288</v>
       </c>
       <c r="G7">
-        <v>1492151629</v>
+        <v>1492237703</v>
       </c>
       <c r="I7" t="s">
         <v>320</v>
@@ -18863,7 +18863,7 @@
         <v>62.0342352</v>
       </c>
       <c r="C8">
-        <v>1492151640</v>
+        <v>1492237718</v>
       </c>
       <c r="D8">
         <v>9.231</v>
@@ -18875,7 +18875,7 @@
         <v>288</v>
       </c>
       <c r="G8">
-        <v>1492151630</v>
+        <v>1492237704</v>
       </c>
       <c r="I8" t="s">
         <v>319</v>
@@ -18901,7 +18901,7 @@
         <v>54.77471999999999</v>
       </c>
       <c r="C9">
-        <v>1492151641</v>
+        <v>1492237719</v>
       </c>
       <c r="D9">
         <v>8.151</v>
@@ -18913,7 +18913,7 @@
         <v>288</v>
       </c>
       <c r="G9">
-        <v>1492151631</v>
+        <v>1492237705</v>
       </c>
       <c r="I9" t="s">
         <v>320</v>
@@ -18939,7 +18939,7 @@
         <v>55.73232000000001</v>
       </c>
       <c r="C10">
-        <v>1492151642</v>
+        <v>1492237720</v>
       </c>
       <c r="D10">
         <v>9.167</v>
@@ -18951,7 +18951,7 @@
         <v>288</v>
       </c>
       <c r="G10">
-        <v>1492151632</v>
+        <v>1492237706</v>
       </c>
       <c r="I10" t="s">
         <v>319</v>
@@ -18977,7 +18977,7 @@
         <v>49.50032</v>
       </c>
       <c r="C11">
-        <v>1492151643</v>
+        <v>1492237721</v>
       </c>
       <c r="D11">
         <v>8.141999999999999</v>
@@ -18989,7 +18989,7 @@
         <v>288</v>
       </c>
       <c r="G11">
-        <v>1492151633</v>
+        <v>1492237707</v>
       </c>
       <c r="I11" t="s">
         <v>320</v>
@@ -19015,7 +19015,7 @@
         <v>48.90732</v>
       </c>
       <c r="C12">
-        <v>1492151644</v>
+        <v>1492237722</v>
       </c>
       <c r="D12">
         <v>9.124000000000001</v>
@@ -19027,7 +19027,7 @@
         <v>288</v>
       </c>
       <c r="G12">
-        <v>1492151634</v>
+        <v>1492237708</v>
       </c>
       <c r="I12" t="s">
         <v>319</v>
@@ -19053,7 +19053,7 @@
         <v>46.0311708</v>
       </c>
       <c r="C13">
-        <v>1492151645</v>
+        <v>1492237723</v>
       </c>
       <c r="D13">
         <v>8.587999999999999</v>
@@ -19065,7 +19065,7 @@
         <v>288</v>
       </c>
       <c r="G13">
-        <v>1492151635</v>
+        <v>1492237709</v>
       </c>
       <c r="I13" t="s">
         <v>320</v>
@@ -19091,7 +19091,7 @@
         <v>45.486</v>
       </c>
       <c r="C14">
-        <v>1492151646</v>
+        <v>1492237724</v>
       </c>
       <c r="D14">
         <v>9.975</v>
@@ -19103,7 +19103,7 @@
         <v>288</v>
       </c>
       <c r="G14">
-        <v>1492151636</v>
+        <v>1492237710</v>
       </c>
       <c r="I14" t="s">
         <v>319</v>
@@ -19129,7 +19129,7 @@
         <v>40.85076</v>
       </c>
       <c r="C15">
-        <v>1492151647</v>
+        <v>1492237725</v>
       </c>
       <c r="D15">
         <v>8.958</v>
@@ -19141,7 +19141,7 @@
         <v>288</v>
       </c>
       <c r="G15">
-        <v>1492151637</v>
+        <v>1492237711</v>
       </c>
       <c r="I15" t="s">
         <v>320</v>
@@ -19167,7 +19167,7 @@
         <v>40.64676000000001</v>
       </c>
       <c r="C16">
-        <v>1492151648</v>
+        <v>1492237726</v>
       </c>
       <c r="D16">
         <v>9.587</v>
@@ -19179,7 +19179,7 @@
         <v>288</v>
       </c>
       <c r="G16">
-        <v>1492151638</v>
+        <v>1492237712</v>
       </c>
       <c r="I16" t="s">
         <v>319</v>
@@ -19205,7 +19205,7 @@
         <v>36.53396000000001</v>
       </c>
       <c r="C17">
-        <v>1492151649</v>
+        <v>1492237727</v>
       </c>
       <c r="D17">
         <v>8.617000000000001</v>
@@ -19217,7 +19217,7 @@
         <v>288</v>
       </c>
       <c r="G17">
-        <v>1492151639</v>
+        <v>1492237713</v>
       </c>
       <c r="I17" t="s">
         <v>320</v>
@@ -19243,7 +19243,7 @@
         <v>36.08472000000001</v>
       </c>
       <c r="C18">
-        <v>1492151650</v>
+        <v>1492237728</v>
       </c>
       <c r="D18">
         <v>9.597</v>
@@ -19255,7 +19255,7 @@
         <v>288</v>
       </c>
       <c r="G18">
-        <v>1492151640</v>
+        <v>1492237714</v>
       </c>
       <c r="I18" t="s">
         <v>319</v>
@@ -19281,7 +19281,7 @@
         <v>33.86256</v>
       </c>
       <c r="C19">
-        <v>1492151651</v>
+        <v>1492237729</v>
       </c>
       <c r="D19">
         <v>9.006</v>
@@ -19293,7 +19293,7 @@
         <v>288</v>
       </c>
       <c r="G19">
-        <v>1492151641</v>
+        <v>1492237715</v>
       </c>
       <c r="I19" t="s">
         <v>320</v>
@@ -19319,7 +19319,7 @@
         <v>34.0452</v>
       </c>
       <c r="C20">
-        <v>1492151652</v>
+        <v>1492237730</v>
       </c>
       <c r="D20">
         <v>10.133</v>
@@ -19331,7 +19331,7 @@
         <v>288</v>
       </c>
       <c r="G20">
-        <v>1492151642</v>
+        <v>1492237716</v>
       </c>
       <c r="I20" t="s">
         <v>319</v>
@@ -19357,7 +19357,7 @@
         <v>30.324</v>
       </c>
       <c r="C21">
-        <v>1492151653</v>
+        <v>1492237731</v>
       </c>
       <c r="D21">
         <v>9.025</v>
@@ -19369,7 +19369,7 @@
         <v>288</v>
       </c>
       <c r="G21">
-        <v>1492151643</v>
+        <v>1492237717</v>
       </c>
       <c r="I21" t="s">
         <v>320</v>

</xml_diff>